<commit_message>
added description 2 - princeton
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>City</t>
   </si>
@@ -31,6 +31,21 @@
   </si>
   <si>
     <t>yjyservices</t>
+  </si>
+  <si>
+    <t>Princton</t>
+  </si>
+  <si>
+    <t>BucksLocks</t>
+  </si>
+  <si>
+    <t>phone verify</t>
+  </si>
+  <si>
+    <t>Bucks locks</t>
+  </si>
+  <si>
+    <t>My 718 phone</t>
   </si>
 </sst>
 </file>
@@ -362,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,8 +395,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -390,6 +408,23 @@
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>